<commit_message>
burndown chart and classDiagram
</commit_message>
<xml_diff>
--- a/BurndownChart.xlsx
+++ b/BurndownChart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\SEP2_eNTe\SEP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5D7DA84F-0C32-43B2-81BB-4D31F778757A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -23,8 +24,19 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>ideal</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1209,16 +1221,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1542,16 +1554,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>91</v>
       </c>
@@ -1559,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>84</v>
       </c>
@@ -1567,7 +1587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>77</v>
       </c>
@@ -1575,7 +1595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>70</v>
       </c>
@@ -1583,7 +1603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>63</v>
       </c>
@@ -1591,7 +1611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>56</v>
       </c>
@@ -1599,7 +1619,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>49</v>
       </c>
@@ -1607,7 +1627,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>42</v>
       </c>
@@ -1615,7 +1635,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>35</v>
       </c>
@@ -1623,7 +1643,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>28</v>
       </c>
@@ -1631,7 +1651,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>21</v>
       </c>
@@ -1639,7 +1659,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>14</v>
       </c>
@@ -1647,7 +1667,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1655,7 +1675,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Burndown chart, closer to the final version
</commit_message>
<xml_diff>
--- a/BurndownChart.xlsx
+++ b/BurndownChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\SEP2_eNTe\SEP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D08F4075-A5EE-4B03-A513-B7B6C8551EC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D99F4202-D017-43F0-94CE-13ED7FB142AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ideal</t>
   </si>
@@ -47,6 +46,12 @@
   </si>
   <si>
     <t>Ideal without extra</t>
+  </si>
+  <si>
+    <t>noooo, almost</t>
+  </si>
+  <si>
+    <t>18 for the reports+ sth</t>
   </si>
 </sst>
 </file>
@@ -271,9 +276,6 @@
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
@@ -325,9 +327,6 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -476,9 +475,6 @@
                 <c:pt idx="13">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>91</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -570,9 +566,6 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
@@ -658,9 +651,6 @@
                   <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
@@ -1866,10 +1856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2177,10 +2167,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>43255</v>
+        <v>43258</v>
       </c>
       <c r="B15">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2196,24 +2186,131 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>43174</v>
+      </c>
+      <c r="C19">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>43181</v>
+      </c>
+      <c r="C20">
+        <f>C19-10</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>43188</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:C28" si="0">C20-10</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43195</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>43202</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>43209</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>43216</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>43223</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>43230</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>43237</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>43244</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>43251</v>
+      </c>
+      <c r="C30">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>43258</v>
       </c>
-      <c r="B16">
-        <v>91</v>
-      </c>
-      <c r="C16">
+      <c r="C31">
         <v>0</v>
       </c>
-      <c r="E16">
-        <v>91</v>
-      </c>
-      <c r="F16">
-        <v>53</v>
-      </c>
-      <c r="G16">
-        <v>53</v>
-      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor change in the burndown chart
</commit_message>
<xml_diff>
--- a/BurndownChart.xlsx
+++ b/BurndownChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\SEP2_eNTe\SEP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C71AC24F-8A38-48D1-B772-A6E30FEC7FB8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B22ED347-E9A2-4A92-9F78-0BE2C18CAC9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -908,7 +908,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>Sum of Task Estimates (days)</a:t>
+                  <a:t>Sum of Task Estimates</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1947,7 +1947,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>